<commit_message>
display temaplte and tests
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/display_template.xlsx
+++ b/Projects/PEPSICOUK/Data/display_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$104</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
@@ -20,8 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$104</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$104</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="115">
   <si>
     <t xml:space="preserve">Display Name</t>
   </si>
@@ -206,7 +205,7 @@
     <t xml:space="preserve">n. Stacking Tray</t>
   </si>
   <si>
-    <t xml:space="preserve">o.  Box Display</t>
+    <t xml:space="preserve">o. Box Display</t>
   </si>
   <si>
     <t xml:space="preserve">q. Pack Display</t>
@@ -338,16 +337,16 @@
     <t xml:space="preserve">Tesco goal post display</t>
   </si>
   <si>
-    <t xml:space="preserve">Head Office Gondola End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremental Gondola End</t>
+    <t xml:space="preserve">HO Agreed Gondola End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non HO Gondola End</t>
   </si>
   <si>
     <t xml:space="preserve">Case Display</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-HO Agreed shelf display</t>
+    <t xml:space="preserve">Non HO Agreed shelf display</t>
   </si>
   <si>
     <t xml:space="preserve">Shelved Side stack</t>
@@ -375,6 +374,9 @@
   </si>
   <si>
     <t xml:space="preserve">Asda in Fixture (FTG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morrisons FTG Kit (FTG)</t>
   </si>
 </sst>
 </file>
@@ -490,7 +492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,6 +519,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -600,22 +606,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2695,8 +2700,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="105" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F104"/>
+  <autoFilter ref="A1:F105"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>